<commit_message>
Volt VAR WATT working
</commit_message>
<xml_diff>
--- a/ProjectFiles/HECO/PyDSS Settings/HP-VV-VW/ExportLists/ExportMode-byClass.xlsx
+++ b/ProjectFiles/HECO/PyDSS Settings/HP-VV-VW/ExportLists/ExportMode-byClass.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Class</t>
   </si>
@@ -27,22 +27,16 @@
     <t>Property</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
     <t>Powers</t>
   </si>
   <si>
-    <t>Loads</t>
+    <t>PVsystems</t>
   </si>
   <si>
-    <t>NumPhases</t>
+    <t>VoltagesMagAng</t>
   </si>
   <si>
-    <t>kW</t>
-  </si>
-  <si>
-    <t>PVsystems</t>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -221,12 +215,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{04990430-CE08-441C-B2BD-2AFFEB72CF57}" name="Table1" displayName="Table1" ref="A2:C4" insertRowShift="1" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A2:C4" xr:uid="{E3360F6F-2B86-4F28-B72A-A82F0B4B3ACF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{04990430-CE08-441C-B2BD-2AFFEB72CF57}" name="Table1" displayName="Table1" ref="A2:C3" insertRowShift="1" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A2:C3" xr:uid="{E3360F6F-2B86-4F28-B72A-A82F0B4B3ACF}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{3619F9E2-CABB-4374-90B5-6CD83340E6A7}" name="Class" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{B115F4B2-93D8-4543-9D4B-E76870DA17CA}" name="Property" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{BAF9E099-640A-4A9F-AEC2-96383B7D9258}" name="Column1" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{B115F4B2-93D8-4543-9D4B-E76870DA17CA}" name="Column1" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{385E6A20-352A-449C-AA92-06EDF9B9E6D1}" name="Property" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -495,58 +489,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>